<commit_message>
Site updated: 2017-08-15 15:02:19
</commit_message>
<xml_diff>
--- a/data/分布式定时任务对比.xlsx
+++ b/data/分布式定时任务对比.xlsx
@@ -592,7 +592,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -603,7 +603,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -653,6 +652,15 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -663,16 +671,13 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -977,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D2" sqref="A1:D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -989,31 +994,31 @@
     <col min="4" max="4" width="29" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" s="29" customFormat="1" ht="23.25" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.25" customHeight="1">
+    <row r="2" spans="1:4" ht="16.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="24" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1021,177 +1026,177 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="23"/>
+      <c r="D3" s="25"/>
     </row>
     <row r="4" spans="1:4" ht="17.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="23"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="25"/>
     </row>
     <row r="5" spans="1:4" ht="17.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="25"/>
     </row>
     <row r="6" spans="1:4" ht="54">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="23"/>
+      <c r="D6" s="25"/>
     </row>
     <row r="7" spans="1:4" ht="31.5">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="23"/>
+      <c r="D7" s="25"/>
     </row>
     <row r="8" spans="1:4" ht="42.75">
       <c r="A8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="23"/>
+      <c r="D8" s="25"/>
     </row>
     <row r="9" spans="1:4" ht="42.75">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="25"/>
     </row>
     <row r="10" spans="1:4" ht="33">
       <c r="A10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="23"/>
+      <c r="D10" s="25"/>
     </row>
     <row r="11" spans="1:4" ht="99.75">
       <c r="A11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="23"/>
+      <c r="D11" s="25"/>
     </row>
     <row r="12" spans="1:4" ht="17.25">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="23"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="25"/>
     </row>
     <row r="13" spans="1:4" ht="17.25">
       <c r="A13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="23"/>
+      <c r="D13" s="25"/>
     </row>
     <row r="14" spans="1:4" ht="27">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="23"/>
+      <c r="D14" s="25"/>
     </row>
     <row r="15" spans="1:4" ht="162" customHeight="1">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="23"/>
+      <c r="D15" s="25"/>
     </row>
     <row r="16" spans="1:4" ht="108">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="23"/>
+      <c r="D16" s="25"/>
     </row>
     <row r="17" spans="1:4" ht="81">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="24"/>
+      <c r="D17" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>